<commit_message>
V 1.0.1: Update Add download control
</commit_message>
<xml_diff>
--- a/RETPER ARBA AGIP.xlsx
+++ b/RETPER ARBA AGIP.xlsx
@@ -1,22 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\BOT RETPER IIBB ARBA AGIP\RETPER ARBA y AGIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8EF1238-76A5-45A6-9946-4E52FBC43538}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11204B2F-54C5-4AAB-80B6-E80A9C7D1DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Clientes" sheetId="1" r:id="rId1"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId2"/>
+  </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$S$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
   <si>
     <t>CLIENTES</t>
   </si>
@@ -117,6 +120,12 @@
   </si>
   <si>
     <t>Fila</t>
+  </si>
+  <si>
+    <t>Resultado ARBA</t>
+  </si>
+  <si>
+    <t>Resultado AGIP</t>
   </si>
 </sst>
 </file>
@@ -245,6 +254,66 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <xxl21:alternateUrls>
+      <xxl21:absoluteUrl r:id="rId2"/>
+    </xxl21:alternateUrls>
+    <sheetNames>
+      <sheetName val="ARBA"/>
+      <sheetName val="AGIP"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Fila</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Resultado</v>
+          </cell>
+        </row>
+        <row r="5">
+          <cell r="A5" t="str">
+            <v>5</v>
+          </cell>
+          <cell r="B5" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+        <row r="6">
+          <cell r="A6" t="str">
+            <v>6</v>
+          </cell>
+          <cell r="B6" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+        <row r="7">
+          <cell r="A7" t="str">
+            <v>7</v>
+          </cell>
+          <cell r="B7" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+      </sheetData>
+      <sheetData sheetId="1">
+        <row r="1">
+          <cell r="A1" t="str">
+            <v>Fila</v>
+          </cell>
+          <cell r="B1" t="str">
+            <v>Resultado</v>
+          </cell>
+        </row>
+      </sheetData>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -568,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q13"/>
+  <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="L5" sqref="L5"/>
+    <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="V5" sqref="V5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -588,7 +657,7 @@
     <col min="12" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -640,8 +709,14 @@
       <c r="Q1" s="8" t="s">
         <v>26</v>
       </c>
+      <c r="R1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="S1" s="8" t="s">
+        <v>28</v>
+      </c>
     </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -671,15 +746,15 @@
         <v>44896</v>
       </c>
       <c r="K2" s="10" t="str">
-        <f t="shared" ref="K2:K13" si="0">TEXT(J2,"AAAA/MM")</f>
+        <f t="shared" ref="K2:K14" si="0">TEXT(J2,"AAAA/MM")</f>
         <v>2022/12</v>
       </c>
       <c r="L2" s="10">
-        <f t="shared" ref="L2:L10" si="1">YEAR(J2)</f>
+        <f t="shared" ref="L2:L11" si="1">YEAR(J2)</f>
         <v>2022</v>
       </c>
       <c r="M2" s="10">
-        <f t="shared" ref="M2:M10" si="2">MONTH(J2)</f>
+        <f t="shared" ref="M2:M11" si="2">MONTH(J2)</f>
         <v>12</v>
       </c>
       <c r="N2" s="10">
@@ -694,12 +769,20 @@
         <f>CONCATENATE(B2," - ",TEXT(J2,"AAAAMM")," - ",IF(F2="",A2,F2))</f>
         <v>20045175333 - 202212 - Valletta Ediciones SRL</v>
       </c>
-      <c r="Q2" s="10">
-        <f>ROW(A2)</f>
+      <c r="Q2" s="10" t="str">
+        <f>TEXT(ROW(A2),"0")</f>
         <v>2</v>
       </c>
+      <c r="R2" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q2,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S2" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q2,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -718,11 +801,11 @@
         <v>16</v>
       </c>
       <c r="H3" s="11" t="str">
-        <f t="shared" ref="H3:H13" si="3">G3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;L3&amp;"\"&amp;TEXT(M3,"00")&amp;"\"</f>
+        <f t="shared" ref="H3:H14" si="3">G3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;L3&amp;"\"&amp;TEXT(M3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2023\01\</v>
       </c>
       <c r="I3" s="11" t="str">
-        <f t="shared" ref="I3:I13" si="4">G3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;L3&amp;"\"&amp;TEXT(M3,"00")&amp;"\"</f>
+        <f t="shared" ref="I3:I14" si="4">G3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;L3&amp;"\"&amp;TEXT(M3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2023\01\</v>
       </c>
       <c r="J3" s="9">
@@ -741,23 +824,31 @@
         <v>1</v>
       </c>
       <c r="N3" s="10">
-        <f t="shared" ref="N3:N13" si="5">IF(B3=B2,0,1)</f>
+        <f t="shared" ref="N3:N14" si="5">IF(B3=B2,0,1)</f>
         <v>0</v>
       </c>
       <c r="O3" s="10">
-        <f t="shared" ref="O3:O13" si="6">IF(B4=B3,0,1)</f>
+        <f t="shared" ref="O3:O14" si="6">IF(B4=B3,0,1)</f>
         <v>0</v>
       </c>
       <c r="P3" s="10" t="str">
-        <f t="shared" ref="P3:P13" si="7">CONCATENATE(B3," - ",TEXT(J3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
+        <f t="shared" ref="P3:P14" si="7">CONCATENATE(B3," - ",TEXT(J3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
         <v>20045175333 - 202301 - Valletta Ediciones SRL</v>
       </c>
-      <c r="Q3" s="10">
-        <f t="shared" ref="Q3:Q13" si="8">ROW(A3)</f>
+      <c r="Q3" s="10" t="str">
+        <f t="shared" ref="Q3:Q14" si="8">TEXT(ROW(A3),"0")</f>
         <v>3</v>
       </c>
+      <c r="R3" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q3,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S3" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q3,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -810,12 +901,20 @@
         <f t="shared" si="7"/>
         <v>20045175333 - 202302 - Valletta Ediciones SRL</v>
       </c>
-      <c r="Q4" s="10">
+      <c r="Q4" s="10" t="str">
         <f t="shared" si="8"/>
         <v>4</v>
       </c>
+      <c r="R4" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q4,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S4" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q4,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -866,12 +965,20 @@
         <f t="shared" si="7"/>
         <v>20252348264 - 202212 - Schmeigel Alejandro Daniel</v>
       </c>
-      <c r="Q5" s="10">
+      <c r="Q5" s="10" t="str">
         <f t="shared" si="8"/>
         <v>5</v>
       </c>
+      <c r="R5" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q5,[1]ARBA!$A:$B,2,0),"")</f>
+        <v>OK</v>
+      </c>
+      <c r="S5" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q5,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -888,26 +995,26 @@
         <v>16</v>
       </c>
       <c r="H6" s="11" t="str">
-        <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\01\</v>
+        <f t="shared" ref="H6" si="9">G6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;L6&amp;"\"&amp;TEXT(M6,"00")&amp;"\"</f>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2007\01\</v>
       </c>
       <c r="I6" s="11" t="str">
-        <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\01\</v>
+        <f t="shared" ref="I6" si="10">G6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;L6&amp;"\"&amp;TEXT(M6,"00")&amp;"\"</f>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2007\01\</v>
       </c>
       <c r="J6" s="9">
-        <v>44927</v>
+        <v>39083</v>
       </c>
       <c r="K6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>2023/01</v>
+        <f t="shared" ref="K6" si="11">TEXT(J6,"AAAA/MM")</f>
+        <v>2007/01</v>
       </c>
       <c r="L6" s="10">
-        <f t="shared" si="1"/>
-        <v>2023</v>
+        <f t="shared" ref="L6" si="12">YEAR(J6)</f>
+        <v>2007</v>
       </c>
       <c r="M6" s="10">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="M6" si="13">MONTH(J6)</f>
         <v>1</v>
       </c>
       <c r="N6" s="10">
@@ -919,15 +1026,23 @@
         <v>0</v>
       </c>
       <c r="P6" s="10" t="str">
-        <f t="shared" si="7"/>
-        <v>20252348264 - 202301 - Schmeigel Alejandro Daniel</v>
-      </c>
-      <c r="Q6" s="10">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="P6" si="14">CONCATENATE(B6," - ",TEXT(J6,"AAAAMM")," - ",IF(F6="",A6,F6))</f>
+        <v>20252348264 - 200701 - Schmeigel Alejandro Daniel</v>
+      </c>
+      <c r="Q6" s="10" t="str">
+        <f t="shared" ref="Q6" si="15">TEXT(ROW(A6),"0")</f>
         <v>6</v>
       </c>
+      <c r="R6" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q6,[1]ARBA!$A:$B,2,0),"")</f>
+        <v>OK</v>
+      </c>
+      <c r="S6" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q6,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -945,18 +1060,18 @@
       </c>
       <c r="H7" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\02\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\01\</v>
       </c>
       <c r="I7" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\02\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\01\</v>
       </c>
       <c r="J7" s="9">
-        <v>44958</v>
+        <v>44927</v>
       </c>
       <c r="K7" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2023/02</v>
+        <v>2023/01</v>
       </c>
       <c r="L7" s="10">
         <f t="shared" si="1"/>
@@ -964,7 +1079,7 @@
       </c>
       <c r="M7" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N7" s="10">
         <f t="shared" si="5"/>
@@ -972,74 +1087,90 @@
       </c>
       <c r="O7" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P7" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>20252348264 - 202302 - Schmeigel Alejandro Daniel</v>
-      </c>
-      <c r="Q7" s="10">
+        <v>20252348264 - 202301 - Schmeigel Alejandro Daniel</v>
+      </c>
+      <c r="Q7" s="10" t="str">
         <f t="shared" si="8"/>
         <v>7</v>
       </c>
+      <c r="R7" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q7,[1]ARBA!$A:$B,2,0),"")</f>
+        <v>OK</v>
+      </c>
+      <c r="S7" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q7,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B8" s="2">
-        <v>27232095984</v>
+        <v>20252348264</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4" t="s">
-        <v>7</v>
-      </c>
+      <c r="D8" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E8" s="4"/>
       <c r="F8" s="2"/>
       <c r="G8" s="12" t="s">
         <v>16</v>
       </c>
       <c r="H8" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2022\12\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\02\</v>
       </c>
       <c r="I8" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2022\12\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\02\</v>
       </c>
       <c r="J8" s="9">
-        <v>44896</v>
+        <v>44958</v>
       </c>
       <c r="K8" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2022/12</v>
+        <v>2023/02</v>
       </c>
       <c r="L8" s="10">
         <f t="shared" si="1"/>
-        <v>2022</v>
+        <v>2023</v>
       </c>
       <c r="M8" s="10">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="N8" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O8" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P8" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>27232095984 - 202212 - Mendoza Vanesa Rosana</v>
-      </c>
-      <c r="Q8" s="10">
+        <v>20252348264 - 202302 - Schmeigel Alejandro Daniel</v>
+      </c>
+      <c r="Q8" s="10" t="str">
         <f t="shared" si="8"/>
         <v>8</v>
       </c>
+      <c r="R8" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q8,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S8" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q8,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1057,30 +1188,30 @@
       </c>
       <c r="H9" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\01\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2022\12\</v>
       </c>
       <c r="I9" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\01\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2022\12\</v>
       </c>
       <c r="J9" s="9">
-        <v>44927</v>
+        <v>44896</v>
       </c>
       <c r="K9" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2023/01</v>
+        <v>2022/12</v>
       </c>
       <c r="L9" s="10">
         <f t="shared" si="1"/>
-        <v>2023</v>
+        <v>2022</v>
       </c>
       <c r="M9" s="10">
         <f t="shared" si="2"/>
-        <v>1</v>
+        <v>12</v>
       </c>
       <c r="N9" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O9" s="10">
         <f t="shared" si="6"/>
@@ -1088,14 +1219,22 @@
       </c>
       <c r="P9" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>27232095984 - 202301 - Mendoza Vanesa Rosana</v>
-      </c>
-      <c r="Q9" s="10">
+        <v>27232095984 - 202212 - Mendoza Vanesa Rosana</v>
+      </c>
+      <c r="Q9" s="10" t="str">
         <f t="shared" si="8"/>
         <v>9</v>
       </c>
+      <c r="R9" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q9,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S9" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q9,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1113,18 +1252,18 @@
       </c>
       <c r="H10" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\02\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\01\</v>
       </c>
       <c r="I10" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\02\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\01\</v>
       </c>
       <c r="J10" s="9">
-        <v>44958</v>
+        <v>44927</v>
       </c>
       <c r="K10" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2023/02</v>
+        <v>2023/01</v>
       </c>
       <c r="L10" s="10">
         <f t="shared" si="1"/>
@@ -1132,7 +1271,7 @@
       </c>
       <c r="M10" s="10">
         <f t="shared" si="2"/>
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N10" s="10">
         <f t="shared" si="5"/>
@@ -1140,28 +1279,36 @@
       </c>
       <c r="O10" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P10" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>27232095984 - 202302 - Mendoza Vanesa Rosana</v>
-      </c>
-      <c r="Q10" s="10">
+        <v>27232095984 - 202301 - Mendoza Vanesa Rosana</v>
+      </c>
+      <c r="Q10" s="10" t="str">
         <f t="shared" si="8"/>
         <v>10</v>
       </c>
+      <c r="R10" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q10,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S10" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q10,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="B11" s="2">
-        <v>20164974589</v>
-      </c>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2" t="s">
-        <v>19</v>
+        <v>27232095984</v>
+      </c>
+      <c r="C11" s="3"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4" t="s">
+        <v>7</v>
       </c>
       <c r="F11" s="2"/>
       <c r="G11" s="12" t="s">
@@ -1169,45 +1316,53 @@
       </c>
       <c r="H11" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2022\12\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\02\</v>
       </c>
       <c r="I11" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2022\12\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\02\</v>
       </c>
       <c r="J11" s="9">
-        <v>44896</v>
+        <v>44958</v>
       </c>
       <c r="K11" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2022/12</v>
+        <v>2023/02</v>
       </c>
       <c r="L11" s="10">
-        <f t="shared" ref="L11:L13" si="9">YEAR(J11)</f>
-        <v>2022</v>
+        <f t="shared" si="1"/>
+        <v>2023</v>
       </c>
       <c r="M11" s="10">
-        <f t="shared" ref="M11:M13" si="10">MONTH(J11)</f>
-        <v>12</v>
+        <f t="shared" si="2"/>
+        <v>2</v>
       </c>
       <c r="N11" s="10">
         <f t="shared" si="5"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="O11" s="10">
         <f t="shared" si="6"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="P11" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>20164974589 - 202212 - Garay Sergio Edgardo</v>
-      </c>
-      <c r="Q11" s="10">
+        <v>27232095984 - 202302 - Mendoza Vanesa Rosana</v>
+      </c>
+      <c r="Q11" s="10" t="str">
         <f t="shared" si="8"/>
         <v>11</v>
       </c>
+      <c r="R11" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q11,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S11" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q11,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1225,30 +1380,30 @@
       </c>
       <c r="H12" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\01\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2022\12\</v>
       </c>
       <c r="I12" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\01\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2022\12\</v>
       </c>
       <c r="J12" s="9">
-        <v>44927</v>
+        <v>44896</v>
       </c>
       <c r="K12" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2023/01</v>
+        <v>2022/12</v>
       </c>
       <c r="L12" s="10">
-        <f t="shared" si="9"/>
-        <v>2023</v>
+        <f t="shared" ref="L12:L14" si="16">YEAR(J12)</f>
+        <v>2022</v>
       </c>
       <c r="M12" s="10">
-        <f t="shared" si="10"/>
-        <v>1</v>
+        <f t="shared" ref="M12:M14" si="17">MONTH(J12)</f>
+        <v>12</v>
       </c>
       <c r="N12" s="10">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="O12" s="10">
         <f t="shared" si="6"/>
@@ -1256,14 +1411,22 @@
       </c>
       <c r="P12" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>20164974589 - 202301 - Garay Sergio Edgardo</v>
-      </c>
-      <c r="Q12" s="10">
+        <v>20164974589 - 202212 - Garay Sergio Edgardo</v>
+      </c>
+      <c r="Q12" s="10" t="str">
         <f t="shared" si="8"/>
         <v>12</v>
       </c>
+      <c r="R12" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q12,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S12" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q12,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1281,26 +1444,26 @@
       </c>
       <c r="H13" s="11" t="str">
         <f t="shared" si="3"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\02\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\01\</v>
       </c>
       <c r="I13" s="11" t="str">
         <f t="shared" si="4"/>
-        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\02\</v>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\01\</v>
       </c>
       <c r="J13" s="9">
-        <v>44958</v>
+        <v>44927</v>
       </c>
       <c r="K13" s="10" t="str">
         <f t="shared" si="0"/>
-        <v>2023/02</v>
+        <v>2023/01</v>
       </c>
       <c r="L13" s="10">
-        <f t="shared" si="9"/>
+        <f t="shared" si="16"/>
         <v>2023</v>
       </c>
       <c r="M13" s="10">
-        <f t="shared" si="10"/>
-        <v>2</v>
+        <f t="shared" si="17"/>
+        <v>1</v>
       </c>
       <c r="N13" s="10">
         <f t="shared" si="5"/>
@@ -1308,23 +1471,91 @@
       </c>
       <c r="O13" s="10">
         <f t="shared" si="6"/>
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="P13" s="10" t="str">
         <f t="shared" si="7"/>
-        <v>20164974589 - 202302 - Garay Sergio Edgardo</v>
-      </c>
-      <c r="Q13" s="10">
+        <v>20164974589 - 202301 - Garay Sergio Edgardo</v>
+      </c>
+      <c r="Q13" s="10" t="str">
         <f t="shared" si="8"/>
         <v>13</v>
       </c>
+      <c r="R13" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q13,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S13" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q13,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B14" s="2">
+        <v>20164974589</v>
+      </c>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="11" t="str">
+        <f t="shared" si="3"/>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\02\</v>
+      </c>
+      <c r="I14" s="11" t="str">
+        <f t="shared" si="4"/>
+        <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\02\</v>
+      </c>
+      <c r="J14" s="9">
+        <v>44958</v>
+      </c>
+      <c r="K14" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>2023/02</v>
+      </c>
+      <c r="L14" s="10">
+        <f t="shared" si="16"/>
+        <v>2023</v>
+      </c>
+      <c r="M14" s="10">
+        <f t="shared" si="17"/>
+        <v>2</v>
+      </c>
+      <c r="N14" s="10">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="O14" s="10">
+        <f t="shared" si="6"/>
+        <v>1</v>
+      </c>
+      <c r="P14" s="10" t="str">
+        <f t="shared" si="7"/>
+        <v>20164974589 - 202302 - Garay Sergio Edgardo</v>
+      </c>
+      <c r="Q14" s="10" t="str">
+        <f t="shared" si="8"/>
+        <v>14</v>
+      </c>
+      <c r="R14" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q14,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="S14" s="10" t="str">
+        <f>IFERROR(VLOOKUP(Q14,[1]AGIP!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:M1" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M10">
-      <sortCondition ref="B1"/>
-    </sortState>
-  </autoFilter>
+  <autoFilter ref="A1:S14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4">
     <sortCondition ref="A2"/>
   </sortState>

</xml_diff>

<commit_message>
RET AGIP en proceso
</commit_message>
<xml_diff>
--- a/RETPER ARBA AGIP.xlsx
+++ b/RETPER ARBA AGIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\BOT RETPER IIBB ARBA AGIP\RETPER ARBA y AGIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11204B2F-54C5-4AAB-80B6-E80A9C7D1DC9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BCFB540-60E4-4879-A570-CFC4D2B48EB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$S$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$T$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="30">
   <si>
     <t>CLIENTES</t>
   </si>
@@ -126,6 +126,9 @@
   </si>
   <si>
     <t>Resultado AGIP</t>
+  </si>
+  <si>
+    <t>Representante AGIP</t>
   </si>
 </sst>
 </file>
@@ -231,7 +234,6 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment shrinkToFit="1"/>
@@ -239,6 +241,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,10 +640,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:S14"/>
+  <dimension ref="A1:T14"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="V5" sqref="V5"/>
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -650,14 +653,14 @@
     <col min="3" max="3" width="21.28515625" style="1" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="25.85546875" style="1" customWidth="1"/>
-    <col min="7" max="9" width="19.7109375" style="1" customWidth="1"/>
-    <col min="10" max="10" width="11.42578125" style="1"/>
-    <col min="11" max="11" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="16384" width="11.42578125" style="1"/>
+    <col min="6" max="7" width="25.85546875" style="1" customWidth="1"/>
+    <col min="8" max="10" width="19.7109375" style="1" customWidth="1"/>
+    <col min="11" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -677,46 +680,49 @@
         <v>10</v>
       </c>
       <c r="G1" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -731,58 +737,62 @@
       <c r="F2" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G2" s="12" t="s">
+      <c r="G2" s="7" t="str">
+        <f>IF(F2="","",CONCATENATE(UPPER(F2)," ","[",TEXT(B2,"00-00000000-0"),"]"))</f>
+        <v>VALLETTA EDICIONES SRL [20-04517533-3]</v>
+      </c>
+      <c r="H2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H2" s="11" t="str">
-        <f>G2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\ARBA\"&amp;L2&amp;"\"&amp;TEXT(M2,"00")&amp;"\"</f>
+      <c r="I2" s="10" t="str">
+        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\ARBA\"&amp;M2&amp;"\"&amp;TEXT(N2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="I2" s="11" t="str">
-        <f>G2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\AGIP\"&amp;L2&amp;"\"&amp;TEXT(M2,"00")&amp;"\"</f>
+      <c r="J2" s="10" t="str">
+        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\AGIP\"&amp;M2&amp;"\"&amp;TEXT(N2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="J2" s="9">
+      <c r="K2" s="12">
         <v>44896</v>
       </c>
-      <c r="K2" s="10" t="str">
-        <f t="shared" ref="K2:K14" si="0">TEXT(J2,"AAAA/MM")</f>
-        <v>2022/12</v>
-      </c>
-      <c r="L2" s="10">
-        <f t="shared" ref="L2:L11" si="1">YEAR(J2)</f>
+      <c r="L2" s="9" t="str">
+        <f>TEXT(K2,"MM/AAAA")</f>
+        <v>12/2022</v>
+      </c>
+      <c r="M2" s="9">
+        <f t="shared" ref="M2:M11" si="0">YEAR(K2)</f>
         <v>2022</v>
       </c>
-      <c r="M2" s="10">
-        <f t="shared" ref="M2:M11" si="2">MONTH(J2)</f>
+      <c r="N2" s="9">
+        <f t="shared" ref="N2:N11" si="1">MONTH(K2)</f>
         <v>12</v>
       </c>
-      <c r="N2" s="10">
+      <c r="O2" s="9">
         <f>IF(B2=B1,0,1)</f>
         <v>1</v>
       </c>
-      <c r="O2" s="10">
+      <c r="P2" s="9">
         <f>IF(B3=B2,0,1)</f>
         <v>0</v>
       </c>
-      <c r="P2" s="10" t="str">
-        <f>CONCATENATE(B2," - ",TEXT(J2,"AAAAMM")," - ",IF(F2="",A2,F2))</f>
+      <c r="Q2" s="9" t="str">
+        <f>CONCATENATE(B2," - ",TEXT(K2,"AAAAMM")," - ",IF(F2="",A2,F2))</f>
         <v>20045175333 - 202212 - Valletta Ediciones SRL</v>
       </c>
-      <c r="Q2" s="10" t="str">
+      <c r="R2" s="9" t="str">
         <f>TEXT(ROW(A2),"0")</f>
         <v>2</v>
       </c>
-      <c r="R2" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q2,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S2" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q2,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S2" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R2,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T2" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R2,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -797,58 +807,62 @@
       <c r="F3" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G3" s="12" t="s">
+      <c r="G3" s="7" t="str">
+        <f t="shared" ref="G3:G14" si="2">IF(F3="","",CONCATENATE(UPPER(F3)," ","[",TEXT(B3,"00-00000000-0"),"]"))</f>
+        <v>VALLETTA EDICIONES SRL [20-04517533-3]</v>
+      </c>
+      <c r="H3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H3" s="11" t="str">
-        <f t="shared" ref="H3:H14" si="3">G3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;L3&amp;"\"&amp;TEXT(M3,"00")&amp;"\"</f>
+      <c r="I3" s="10" t="str">
+        <f t="shared" ref="I3:I14" si="3">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;M3&amp;"\"&amp;TEXT(N3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="I3" s="11" t="str">
-        <f t="shared" ref="I3:I14" si="4">G3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;L3&amp;"\"&amp;TEXT(M3,"00")&amp;"\"</f>
+      <c r="J3" s="10" t="str">
+        <f t="shared" ref="J3:J14" si="4">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;M3&amp;"\"&amp;TEXT(N3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="J3" s="9">
+      <c r="K3" s="12">
         <v>44927</v>
       </c>
-      <c r="K3" s="10" t="str">
+      <c r="L3" s="9" t="str">
+        <f t="shared" ref="L3:L14" si="5">TEXT(K3,"MM/AAAA")</f>
+        <v>01/2023</v>
+      </c>
+      <c r="M3" s="9">
         <f t="shared" si="0"/>
-        <v>2023/01</v>
-      </c>
-      <c r="L3" s="10">
+        <v>2023</v>
+      </c>
+      <c r="N3" s="9">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="M3" s="10">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N3" s="10">
-        <f t="shared" ref="N3:N14" si="5">IF(B3=B2,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="O3" s="10">
-        <f t="shared" ref="O3:O14" si="6">IF(B4=B3,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="P3" s="10" t="str">
-        <f t="shared" ref="P3:P14" si="7">CONCATENATE(B3," - ",TEXT(J3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
+      <c r="O3" s="9">
+        <f t="shared" ref="O3:O14" si="6">IF(B3=B2,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="P3" s="9">
+        <f t="shared" ref="P3:P14" si="7">IF(B4=B3,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9" t="str">
+        <f t="shared" ref="Q3:Q14" si="8">CONCATENATE(B3," - ",TEXT(K3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
         <v>20045175333 - 202301 - Valletta Ediciones SRL</v>
       </c>
-      <c r="Q3" s="10" t="str">
-        <f t="shared" ref="Q3:Q14" si="8">TEXT(ROW(A3),"0")</f>
+      <c r="R3" s="9" t="str">
+        <f t="shared" ref="R3:R14" si="9">TEXT(ROW(A3),"0")</f>
         <v>3</v>
       </c>
-      <c r="R3" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q3,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S3" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q3,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S3" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R3,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T3" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R3,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>8</v>
       </c>
@@ -863,58 +877,62 @@
       <c r="F4" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="12" t="s">
+      <c r="G4" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v>VALLETTA EDICIONES SRL [20-04517533-3]</v>
+      </c>
+      <c r="H4" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H4" s="11" t="str">
+      <c r="I4" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="I4" s="11" t="str">
+      <c r="J4" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="J4" s="9">
+      <c r="K4" s="12">
         <v>44958</v>
       </c>
-      <c r="K4" s="10" t="str">
+      <c r="L4" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>02/2023</v>
+      </c>
+      <c r="M4" s="9">
         <f t="shared" si="0"/>
-        <v>2023/02</v>
-      </c>
-      <c r="L4" s="10">
+        <v>2023</v>
+      </c>
+      <c r="N4" s="9">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="M4" s="10">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="N4" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O4" s="10">
+      <c r="O4" s="9">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P4" s="9">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P4" s="10" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q4" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20045175333 - 202302 - Valletta Ediciones SRL</v>
       </c>
-      <c r="Q4" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R4" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="R4" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q4,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S4" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q4,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S4" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R4,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T4" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R4,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -927,58 +945,62 @@
       </c>
       <c r="E5" s="4"/>
       <c r="F5" s="2"/>
-      <c r="G5" s="12" t="s">
+      <c r="G5" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H5" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H5" s="11" t="str">
+      <c r="I5" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="I5" s="11" t="str">
+      <c r="J5" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="J5" s="9">
+      <c r="K5" s="12">
         <v>44896</v>
       </c>
-      <c r="K5" s="10" t="str">
+      <c r="L5" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>12/2022</v>
+      </c>
+      <c r="M5" s="9">
         <f t="shared" si="0"/>
-        <v>2022/12</v>
-      </c>
-      <c r="L5" s="10">
+        <v>2022</v>
+      </c>
+      <c r="N5" s="9">
         <f t="shared" si="1"/>
-        <v>2022</v>
-      </c>
-      <c r="M5" s="10">
-        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N5" s="10">
-        <f t="shared" si="5"/>
+      <c r="O5" s="9">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O5" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P5" s="10" t="str">
+      <c r="P5" s="9">
         <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q5" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20252348264 - 202212 - Schmeigel Alejandro Daniel</v>
       </c>
-      <c r="Q5" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R5" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="R5" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q5,[1]ARBA!$A:$B,2,0),"")</f>
+      <c r="S5" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R5,[1]ARBA!$A:$B,2,0),"")</f>
         <v>OK</v>
       </c>
-      <c r="S5" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q5,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="T5" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R5,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -991,58 +1013,62 @@
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="12" t="s">
+      <c r="G6" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H6" s="11" t="str">
-        <f t="shared" ref="H6" si="9">G6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;L6&amp;"\"&amp;TEXT(M6,"00")&amp;"\"</f>
+      <c r="I6" s="10" t="str">
+        <f t="shared" ref="I6" si="10">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;M6&amp;"\"&amp;TEXT(N6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2007\01\</v>
       </c>
-      <c r="I6" s="11" t="str">
-        <f t="shared" ref="I6" si="10">G6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;L6&amp;"\"&amp;TEXT(M6,"00")&amp;"\"</f>
+      <c r="J6" s="10" t="str">
+        <f t="shared" ref="J6" si="11">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;M6&amp;"\"&amp;TEXT(N6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2007\01\</v>
       </c>
-      <c r="J6" s="9">
+      <c r="K6" s="12">
         <v>39083</v>
       </c>
-      <c r="K6" s="10" t="str">
-        <f t="shared" ref="K6" si="11">TEXT(J6,"AAAA/MM")</f>
-        <v>2007/01</v>
-      </c>
-      <c r="L6" s="10">
-        <f t="shared" ref="L6" si="12">YEAR(J6)</f>
+      <c r="L6" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>01/2007</v>
+      </c>
+      <c r="M6" s="9">
+        <f t="shared" ref="M6" si="12">YEAR(K6)</f>
         <v>2007</v>
       </c>
-      <c r="M6" s="10">
-        <f t="shared" ref="M6" si="13">MONTH(J6)</f>
+      <c r="N6" s="9">
+        <f t="shared" ref="N6" si="13">MONTH(K6)</f>
         <v>1</v>
       </c>
-      <c r="N6" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O6" s="10">
+      <c r="O6" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P6" s="10" t="str">
-        <f t="shared" ref="P6" si="14">CONCATENATE(B6," - ",TEXT(J6,"AAAAMM")," - ",IF(F6="",A6,F6))</f>
+      <c r="P6" s="9">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q6" s="9" t="str">
+        <f t="shared" ref="Q6" si="14">CONCATENATE(B6," - ",TEXT(K6,"AAAAMM")," - ",IF(F6="",A6,F6))</f>
         <v>20252348264 - 200701 - Schmeigel Alejandro Daniel</v>
       </c>
-      <c r="Q6" s="10" t="str">
-        <f t="shared" ref="Q6" si="15">TEXT(ROW(A6),"0")</f>
+      <c r="R6" s="9" t="str">
+        <f t="shared" ref="R6" si="15">TEXT(ROW(A6),"0")</f>
         <v>6</v>
       </c>
-      <c r="R6" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q6,[1]ARBA!$A:$B,2,0),"")</f>
+      <c r="S6" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R6,[1]ARBA!$A:$B,2,0),"")</f>
         <v>OK</v>
       </c>
-      <c r="S6" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q6,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="T6" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R6,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -1055,58 +1081,62 @@
       </c>
       <c r="E7" s="4"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="12" t="s">
+      <c r="G7" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H7" s="11" t="str">
+      <c r="I7" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="I7" s="11" t="str">
+      <c r="J7" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="J7" s="9">
+      <c r="K7" s="12">
         <v>44927</v>
       </c>
-      <c r="K7" s="10" t="str">
+      <c r="L7" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>01/2023</v>
+      </c>
+      <c r="M7" s="9">
         <f t="shared" si="0"/>
-        <v>2023/01</v>
-      </c>
-      <c r="L7" s="10">
+        <v>2023</v>
+      </c>
+      <c r="N7" s="9">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="M7" s="10">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N7" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O7" s="10">
+      <c r="O7" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P7" s="10" t="str">
+      <c r="P7" s="9">
         <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q7" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20252348264 - 202301 - Schmeigel Alejandro Daniel</v>
       </c>
-      <c r="Q7" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R7" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="R7" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q7,[1]ARBA!$A:$B,2,0),"")</f>
+      <c r="S7" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R7,[1]ARBA!$A:$B,2,0),"")</f>
         <v>OK</v>
       </c>
-      <c r="S7" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q7,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="T7" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R7,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>4</v>
       </c>
@@ -1119,58 +1149,62 @@
       </c>
       <c r="E8" s="4"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H8" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H8" s="11" t="str">
+      <c r="I8" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="I8" s="11" t="str">
+      <c r="J8" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="J8" s="9">
+      <c r="K8" s="12">
         <v>44958</v>
       </c>
-      <c r="K8" s="10" t="str">
+      <c r="L8" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>02/2023</v>
+      </c>
+      <c r="M8" s="9">
         <f t="shared" si="0"/>
-        <v>2023/02</v>
-      </c>
-      <c r="L8" s="10">
+        <v>2023</v>
+      </c>
+      <c r="N8" s="9">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="M8" s="10">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="N8" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O8" s="10">
+      <c r="O8" s="9">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P8" s="9">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P8" s="10" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q8" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20252348264 - 202302 - Schmeigel Alejandro Daniel</v>
       </c>
-      <c r="Q8" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R8" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="R8" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q8,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S8" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q8,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S8" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R8,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T8" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R8,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
@@ -1183,58 +1217,62 @@
         <v>7</v>
       </c>
       <c r="F9" s="2"/>
-      <c r="G9" s="12" t="s">
+      <c r="G9" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H9" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H9" s="11" t="str">
+      <c r="I9" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="I9" s="11" t="str">
+      <c r="J9" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="J9" s="9">
+      <c r="K9" s="12">
         <v>44896</v>
       </c>
-      <c r="K9" s="10" t="str">
+      <c r="L9" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>12/2022</v>
+      </c>
+      <c r="M9" s="9">
         <f t="shared" si="0"/>
-        <v>2022/12</v>
-      </c>
-      <c r="L9" s="10">
+        <v>2022</v>
+      </c>
+      <c r="N9" s="9">
         <f t="shared" si="1"/>
-        <v>2022</v>
-      </c>
-      <c r="M9" s="10">
-        <f t="shared" si="2"/>
         <v>12</v>
       </c>
-      <c r="N9" s="10">
-        <f t="shared" si="5"/>
+      <c r="O9" s="9">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O9" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P9" s="10" t="str">
+      <c r="P9" s="9">
         <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q9" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>27232095984 - 202212 - Mendoza Vanesa Rosana</v>
       </c>
-      <c r="Q9" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R9" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="R9" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q9,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S9" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q9,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S9" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R9,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T9" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R9,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -1247,58 +1285,62 @@
         <v>7</v>
       </c>
       <c r="F10" s="2"/>
-      <c r="G10" s="12" t="s">
+      <c r="G10" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H10" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H10" s="11" t="str">
+      <c r="I10" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="I10" s="11" t="str">
+      <c r="J10" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="J10" s="9">
+      <c r="K10" s="12">
         <v>44927</v>
       </c>
-      <c r="K10" s="10" t="str">
+      <c r="L10" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>01/2023</v>
+      </c>
+      <c r="M10" s="9">
         <f t="shared" si="0"/>
-        <v>2023/01</v>
-      </c>
-      <c r="L10" s="10">
+        <v>2023</v>
+      </c>
+      <c r="N10" s="9">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="M10" s="10">
-        <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="N10" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O10" s="10">
+      <c r="O10" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P10" s="10" t="str">
+      <c r="P10" s="9">
         <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q10" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>27232095984 - 202301 - Mendoza Vanesa Rosana</v>
       </c>
-      <c r="Q10" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R10" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="R10" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q10,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S10" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q10,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S10" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R10,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T10" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R10,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -1311,58 +1353,62 @@
         <v>7</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="12" t="s">
+      <c r="G11" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H11" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H11" s="11" t="str">
+      <c r="I11" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="I11" s="11" t="str">
+      <c r="J11" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="J11" s="9">
+      <c r="K11" s="12">
         <v>44958</v>
       </c>
-      <c r="K11" s="10" t="str">
+      <c r="L11" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>02/2023</v>
+      </c>
+      <c r="M11" s="9">
         <f t="shared" si="0"/>
-        <v>2023/02</v>
-      </c>
-      <c r="L11" s="10">
+        <v>2023</v>
+      </c>
+      <c r="N11" s="9">
         <f t="shared" si="1"/>
-        <v>2023</v>
-      </c>
-      <c r="M11" s="10">
-        <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="N11" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O11" s="10">
+      <c r="O11" s="9">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P11" s="9">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P11" s="10" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q11" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>27232095984 - 202302 - Mendoza Vanesa Rosana</v>
       </c>
-      <c r="Q11" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R11" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="R11" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q11,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S11" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q11,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S11" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R11,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T11" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R11,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>18</v>
       </c>
@@ -1375,58 +1421,62 @@
         <v>19</v>
       </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="12" t="s">
+      <c r="G12" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H12" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H12" s="11" t="str">
+      <c r="I12" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="I12" s="11" t="str">
+      <c r="J12" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="J12" s="9">
+      <c r="K12" s="12">
         <v>44896</v>
       </c>
-      <c r="K12" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>2022/12</v>
-      </c>
-      <c r="L12" s="10">
-        <f t="shared" ref="L12:L14" si="16">YEAR(J12)</f>
+      <c r="L12" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>12/2022</v>
+      </c>
+      <c r="M12" s="9">
+        <f t="shared" ref="M12:M14" si="16">YEAR(K12)</f>
         <v>2022</v>
       </c>
-      <c r="M12" s="10">
-        <f t="shared" ref="M12:M14" si="17">MONTH(J12)</f>
+      <c r="N12" s="9">
+        <f t="shared" ref="N12:N14" si="17">MONTH(K12)</f>
         <v>12</v>
       </c>
-      <c r="N12" s="10">
-        <f t="shared" si="5"/>
+      <c r="O12" s="9">
+        <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O12" s="10">
-        <f t="shared" si="6"/>
-        <v>0</v>
-      </c>
-      <c r="P12" s="10" t="str">
+      <c r="P12" s="9">
         <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q12" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20164974589 - 202212 - Garay Sergio Edgardo</v>
       </c>
-      <c r="Q12" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R12" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="R12" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q12,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S12" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q12,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S12" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R12,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T12" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R12,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>18</v>
       </c>
@@ -1439,58 +1489,62 @@
         <v>19</v>
       </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="12" t="s">
+      <c r="G13" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H13" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H13" s="11" t="str">
+      <c r="I13" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="I13" s="11" t="str">
+      <c r="J13" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="J13" s="9">
+      <c r="K13" s="12">
         <v>44927</v>
       </c>
-      <c r="K13" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>2023/01</v>
-      </c>
-      <c r="L13" s="10">
+      <c r="L13" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>01/2023</v>
+      </c>
+      <c r="M13" s="9">
         <f t="shared" si="16"/>
         <v>2023</v>
       </c>
-      <c r="M13" s="10">
+      <c r="N13" s="9">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="N13" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O13" s="10">
+      <c r="O13" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P13" s="10" t="str">
+      <c r="P13" s="9">
         <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="Q13" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20164974589 - 202301 - Garay Sergio Edgardo</v>
       </c>
-      <c r="Q13" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R13" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="R13" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q13,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S13" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q13,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S13" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R13,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T13" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R13,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>18</v>
       </c>
@@ -1503,59 +1557,63 @@
         <v>19</v>
       </c>
       <c r="F14" s="2"/>
-      <c r="G14" s="12" t="s">
+      <c r="G14" s="7" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="H14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H14" s="11" t="str">
+      <c r="I14" s="10" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="I14" s="11" t="str">
+      <c r="J14" s="10" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="J14" s="9">
+      <c r="K14" s="12">
         <v>44958</v>
       </c>
-      <c r="K14" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>2023/02</v>
-      </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9" t="str">
+        <f t="shared" si="5"/>
+        <v>02/2023</v>
+      </c>
+      <c r="M14" s="9">
         <f t="shared" si="16"/>
         <v>2023</v>
       </c>
-      <c r="M14" s="10">
+      <c r="N14" s="9">
         <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="N14" s="10">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-      <c r="O14" s="10">
+      <c r="O14" s="9">
         <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="P14" s="9">
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="P14" s="10" t="str">
-        <f t="shared" si="7"/>
+      <c r="Q14" s="9" t="str">
+        <f t="shared" si="8"/>
         <v>20164974589 - 202302 - Garay Sergio Edgardo</v>
       </c>
-      <c r="Q14" s="10" t="str">
-        <f t="shared" si="8"/>
+      <c r="R14" s="9" t="str">
+        <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="R14" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q14,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
-      <c r="S14" s="10" t="str">
-        <f>IFERROR(VLOOKUP(Q14,[1]AGIP!$A:$B,2,0),"")</f>
+      <c r="S14" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R14,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="T14" s="9" t="str">
+        <f>IFERROR(VLOOKUP(R14,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:S14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:T14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4">
     <sortCondition ref="A2"/>
   </sortState>

</xml_diff>

<commit_message>
V 1.0.2: Bots Funcionales
</commit_message>
<xml_diff>
--- a/RETPER ARBA AGIP.xlsx
+++ b/RETPER ARBA AGIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Agustin Bustos\Desktop\BOT RETPER IIBB ARBA AGIP\RETPER ARBA y AGIP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25D516D3-BD51-4C8B-BC06-7E4C3569CC96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD52F1A9-8C7B-41E5-BE2A-2A1188FC0EF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -236,12 +236,12 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -311,6 +311,54 @@
           </cell>
           <cell r="B4" t="str">
             <v>OK</v>
+          </cell>
+        </row>
+        <row r="9">
+          <cell r="A9" t="str">
+            <v>9</v>
+          </cell>
+          <cell r="B9" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+        <row r="10">
+          <cell r="A10" t="str">
+            <v>10</v>
+          </cell>
+          <cell r="B10" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+        <row r="11">
+          <cell r="A11" t="str">
+            <v>11</v>
+          </cell>
+          <cell r="B11" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+        <row r="12">
+          <cell r="A12" t="str">
+            <v>12</v>
+          </cell>
+          <cell r="B12" t="str">
+            <v>No Hay Retenciones para el Período</v>
+          </cell>
+        </row>
+        <row r="13">
+          <cell r="A13" t="str">
+            <v>13</v>
+          </cell>
+          <cell r="B13" t="str">
+            <v>OK</v>
+          </cell>
+        </row>
+        <row r="14">
+          <cell r="A14" t="str">
+            <v>14</v>
+          </cell>
+          <cell r="B14" t="str">
+            <v>No Hay Retenciones para el Período</v>
           </cell>
         </row>
       </sheetData>
@@ -642,8 +690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -741,18 +789,18 @@
         <f>IF(F2="","",CONCATENATE(UPPER(F2)))</f>
         <v>VALLETTA EDICIONES SRL</v>
       </c>
-      <c r="H2" s="11" t="s">
+      <c r="H2" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="10" t="str">
+      <c r="I2" s="12" t="str">
         <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\ARBA\"&amp;M2&amp;"\"&amp;TEXT(N2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J2" s="10" t="str">
+      <c r="J2" s="12" t="str">
         <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\AGIP\"&amp;M2&amp;"\"&amp;TEXT(N2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K2" s="12">
+      <c r="K2" s="11">
         <v>44896</v>
       </c>
       <c r="L2" s="9" t="str">
@@ -811,18 +859,18 @@
         <f t="shared" ref="G3:G14" si="2">IF(F3="","",CONCATENATE(UPPER(F3)))</f>
         <v>VALLETTA EDICIONES SRL</v>
       </c>
-      <c r="H3" s="11" t="s">
+      <c r="H3" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="10" t="str">
+      <c r="I3" s="12" t="str">
         <f t="shared" ref="I3:I14" si="3">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;M3&amp;"\"&amp;TEXT(N3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J3" s="10" t="str">
+      <c r="J3" s="12" t="str">
         <f t="shared" ref="J3:J14" si="4">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;M3&amp;"\"&amp;TEXT(N3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K3" s="12">
+      <c r="K3" s="11">
         <v>44927</v>
       </c>
       <c r="L3" s="9" t="str">
@@ -881,18 +929,18 @@
         <f t="shared" si="2"/>
         <v>VALLETTA EDICIONES SRL</v>
       </c>
-      <c r="H4" s="11" t="s">
+      <c r="H4" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="10" t="str">
+      <c r="I4" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J4" s="10" t="str">
+      <c r="J4" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Valletta Ediciones SRL\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K4" s="12">
+      <c r="K4" s="11">
         <v>44958</v>
       </c>
       <c r="L4" s="9" t="str">
@@ -949,18 +997,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H5" s="11" t="s">
+      <c r="H5" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I5" s="10" t="str">
+      <c r="I5" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J5" s="10" t="str">
+      <c r="J5" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K5" s="12">
+      <c r="K5" s="11">
         <v>44896</v>
       </c>
       <c r="L5" s="9" t="str">
@@ -1017,18 +1065,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H6" s="11" t="s">
+      <c r="H6" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I6" s="10" t="str">
+      <c r="I6" s="12" t="str">
         <f t="shared" ref="I6" si="10">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;M6&amp;"\"&amp;TEXT(N6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2007\01\</v>
       </c>
-      <c r="J6" s="10" t="str">
+      <c r="J6" s="12" t="str">
         <f t="shared" ref="J6" si="11">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;M6&amp;"\"&amp;TEXT(N6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2007\01\</v>
       </c>
-      <c r="K6" s="12">
+      <c r="K6" s="11">
         <v>39083</v>
       </c>
       <c r="L6" s="9" t="str">
@@ -1085,18 +1133,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="H7" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="10" t="str">
+      <c r="I7" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J7" s="10" t="str">
+      <c r="J7" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K7" s="12">
+      <c r="K7" s="11">
         <v>44927</v>
       </c>
       <c r="L7" s="9" t="str">
@@ -1153,18 +1201,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="H8" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I8" s="10" t="str">
+      <c r="I8" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J8" s="10" t="str">
+      <c r="J8" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Schmeigel Alejandro Daniel\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K8" s="12">
+      <c r="K8" s="11">
         <v>44958</v>
       </c>
       <c r="L8" s="9" t="str">
@@ -1221,18 +1269,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="H9" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="10" t="str">
+      <c r="I9" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J9" s="10" t="str">
+      <c r="J9" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K9" s="12">
+      <c r="K9" s="11">
         <v>44896</v>
       </c>
       <c r="L9" s="9" t="str">
@@ -1269,7 +1317,7 @@
       </c>
       <c r="T9" s="9" t="str">
         <f>IFERROR(VLOOKUP(R9,[1]AGIP!$A:$B,2,0),"")</f>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
@@ -1289,18 +1337,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="H10" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="10" t="str">
+      <c r="I10" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J10" s="10" t="str">
+      <c r="J10" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K10" s="12">
+      <c r="K10" s="11">
         <v>44927</v>
       </c>
       <c r="L10" s="9" t="str">
@@ -1337,7 +1385,7 @@
       </c>
       <c r="T10" s="9" t="str">
         <f>IFERROR(VLOOKUP(R10,[1]AGIP!$A:$B,2,0),"")</f>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="11" spans="1:20" x14ac:dyDescent="0.25">
@@ -1357,18 +1405,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H11" s="11" t="s">
+      <c r="H11" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="10" t="str">
+      <c r="I11" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J11" s="10" t="str">
+      <c r="J11" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Mendoza Vanesa Rosana\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K11" s="12">
+      <c r="K11" s="11">
         <v>44958</v>
       </c>
       <c r="L11" s="9" t="str">
@@ -1405,7 +1453,7 @@
       </c>
       <c r="T11" s="9" t="str">
         <f>IFERROR(VLOOKUP(R11,[1]AGIP!$A:$B,2,0),"")</f>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="12" spans="1:20" x14ac:dyDescent="0.25">
@@ -1425,18 +1473,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H12" s="11" t="s">
+      <c r="H12" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="10" t="str">
+      <c r="I12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J12" s="10" t="str">
+      <c r="J12" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K12" s="12">
+      <c r="K12" s="11">
         <v>44896</v>
       </c>
       <c r="L12" s="9" t="str">
@@ -1473,7 +1521,7 @@
       </c>
       <c r="T12" s="9" t="str">
         <f>IFERROR(VLOOKUP(R12,[1]AGIP!$A:$B,2,0),"")</f>
-        <v/>
+        <v>No Hay Retenciones para el Período</v>
       </c>
     </row>
     <row r="13" spans="1:20" x14ac:dyDescent="0.25">
@@ -1493,18 +1541,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H13" s="11" t="s">
+      <c r="H13" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I13" s="10" t="str">
+      <c r="I13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J13" s="10" t="str">
+      <c r="J13" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K13" s="12">
+      <c r="K13" s="11">
         <v>44927</v>
       </c>
       <c r="L13" s="9" t="str">
@@ -1541,7 +1589,7 @@
       </c>
       <c r="T13" s="9" t="str">
         <f>IFERROR(VLOOKUP(R13,[1]AGIP!$A:$B,2,0),"")</f>
-        <v/>
+        <v>OK</v>
       </c>
     </row>
     <row r="14" spans="1:20" x14ac:dyDescent="0.25">
@@ -1561,18 +1609,18 @@
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H14" s="11" t="s">
+      <c r="H14" s="10" t="s">
         <v>16</v>
       </c>
-      <c r="I14" s="10" t="str">
+      <c r="I14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J14" s="10" t="str">
+      <c r="J14" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Garay Sergio Edgardo\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K14" s="12">
+      <c r="K14" s="11">
         <v>44958</v>
       </c>
       <c r="L14" s="9" t="str">
@@ -1609,7 +1657,7 @@
       </c>
       <c r="T14" s="9" t="str">
         <f>IFERROR(VLOOKUP(R14,[1]AGIP!$A:$B,2,0),"")</f>
-        <v/>
+        <v>No Hay Retenciones para el Período</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fusion Simulate type options
</commit_message>
<xml_diff>
--- a/RETPER ARBA AGIP.xlsx
+++ b/RETPER ARBA AGIP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyecto Uipath\RETPER-IIBB-AGIP-ARBA\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\RETPER-IIBB-AGIP-ARBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2997C825-3585-4304-A2DF-E02B04C895F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21164B4F-2E20-4C85-8063-B8808AD2FDF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$T$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$U$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="29">
   <si>
     <t>CLIENTES</t>
   </si>
@@ -120,6 +120,12 @@
   </si>
   <si>
     <t>Representante SA</t>
+  </si>
+  <si>
+    <t>ST</t>
+  </si>
+  <si>
+    <t>SI</t>
   </si>
 </sst>
 </file>
@@ -287,9 +293,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -327,9 +333,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -362,26 +368,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -414,26 +403,9 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -607,11 +579,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:T14"/>
+  <dimension ref="A1:U14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -621,13 +591,13 @@
     <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
     <col min="6" max="7" width="25.85546875" style="1" customWidth="1"/>
-    <col min="8" max="10" width="19.7109375" style="1" customWidth="1"/>
-    <col min="11" max="11" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="11.42578125" style="1"/>
+    <col min="8" max="11" width="19.7109375" style="1" customWidth="1"/>
+    <col min="12" max="12" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -653,43 +623,46 @@
         <v>11</v>
       </c>
       <c r="I1" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="J1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -711,55 +684,58 @@
       <c r="H2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="12" t="str">
-        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\ARBA\"&amp;M2&amp;"\"&amp;TEXT(N2,"00")&amp;"\"</f>
+      <c r="I2" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="12" t="str">
+        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\ARBA\"&amp;N2&amp;"\"&amp;TEXT(O2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J2" s="12" t="str">
-        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\AGIP\"&amp;M2&amp;"\"&amp;TEXT(N2,"00")&amp;"\"</f>
+      <c r="K2" s="12" t="str">
+        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\AGIP\"&amp;N2&amp;"\"&amp;TEXT(O2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K2" s="11">
+      <c r="L2" s="11">
         <v>44896</v>
       </c>
-      <c r="L2" s="9" t="str">
-        <f>TEXT(K2,"MM/AAAA")</f>
+      <c r="M2" s="9" t="str">
+        <f>TEXT(L2,"MM/AAAA")</f>
         <v>12/2022</v>
       </c>
-      <c r="M2" s="9">
-        <f t="shared" ref="M2:M11" si="0">YEAR(K2)</f>
+      <c r="N2" s="9">
+        <f t="shared" ref="N2:N11" si="0">YEAR(L2)</f>
         <v>2022</v>
       </c>
-      <c r="N2" s="9">
-        <f t="shared" ref="N2:N11" si="1">MONTH(K2)</f>
+      <c r="O2" s="9">
+        <f t="shared" ref="O2:O11" si="1">MONTH(L2)</f>
         <v>12</v>
       </c>
-      <c r="O2" s="9">
+      <c r="P2" s="9">
         <f>IF(B2=B1,0,1)</f>
         <v>1</v>
       </c>
-      <c r="P2" s="9">
+      <c r="Q2" s="9">
         <f>IF(B3=B2,0,1)</f>
         <v>0</v>
       </c>
-      <c r="Q2" s="9" t="str">
-        <f>CONCATENATE(B2," - ",TEXT(K2,"AAAAMM")," - ",IF(F2="",A2,F2))</f>
+      <c r="R2" s="9" t="str">
+        <f>CONCATENATE(B2," - ",TEXT(L2,"AAAAMM")," - ",IF(F2="",A2,F2))</f>
         <v>20000000000 - 202212 - Representante SA</v>
       </c>
-      <c r="R2" s="9" t="str">
+      <c r="S2" s="9" t="str">
         <f>TEXT(ROW(A2),"0")</f>
         <v>2</v>
       </c>
-      <c r="S2" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R2,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T2" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R2,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S2,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U2" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S2,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -781,55 +757,58 @@
       <c r="H3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="12" t="str">
-        <f t="shared" ref="I3:I14" si="3">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;M3&amp;"\"&amp;TEXT(N3,"00")&amp;"\"</f>
+      <c r="I3" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="12" t="str">
+        <f t="shared" ref="J3:J14" si="3">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;N3&amp;"\"&amp;TEXT(O3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J3" s="12" t="str">
-        <f t="shared" ref="J3:J14" si="4">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;M3&amp;"\"&amp;TEXT(N3,"00")&amp;"\"</f>
+      <c r="K3" s="12" t="str">
+        <f t="shared" ref="K3:K14" si="4">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;N3&amp;"\"&amp;TEXT(O3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K3" s="11">
+      <c r="L3" s="11">
         <v>44927</v>
       </c>
-      <c r="L3" s="9" t="str">
-        <f t="shared" ref="L3:L14" si="5">TEXT(K3,"MM/AAAA")</f>
+      <c r="M3" s="9" t="str">
+        <f t="shared" ref="M3:M14" si="5">TEXT(L3,"MM/AAAA")</f>
         <v>01/2023</v>
       </c>
-      <c r="M3" s="9">
+      <c r="N3" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="N3" s="9">
+      <c r="O3" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O3" s="9">
-        <f t="shared" ref="O3:O14" si="6">IF(B3=B2,0,1)</f>
-        <v>0</v>
-      </c>
       <c r="P3" s="9">
-        <f t="shared" ref="P3:P14" si="7">IF(B4=B3,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="Q3" s="9" t="str">
-        <f t="shared" ref="Q3:Q14" si="8">CONCATENATE(B3," - ",TEXT(K3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
+        <f t="shared" ref="P3:P14" si="6">IF(B3=B2,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="Q3" s="9">
+        <f t="shared" ref="Q3:Q14" si="7">IF(B4=B3,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="R3" s="9" t="str">
+        <f t="shared" ref="R3:R14" si="8">CONCATENATE(B3," - ",TEXT(L3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
         <v>20000000000 - 202301 - Representante SA</v>
       </c>
-      <c r="R3" s="9" t="str">
-        <f t="shared" ref="R3:R14" si="9">TEXT(ROW(A3),"0")</f>
+      <c r="S3" s="9" t="str">
+        <f t="shared" ref="S3:S14" si="9">TEXT(ROW(A3),"0")</f>
         <v>3</v>
       </c>
-      <c r="S3" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R3,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T3" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R3,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S3,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U3" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S3,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -851,55 +830,58 @@
       <c r="H4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="12" t="str">
+      <c r="I4" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J4" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J4" s="12" t="str">
+      <c r="K4" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K4" s="11">
+      <c r="L4" s="11">
         <v>44958</v>
       </c>
-      <c r="L4" s="9" t="str">
+      <c r="M4" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="M4" s="9">
+      <c r="N4" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="N4" s="9">
+      <c r="O4" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q4" s="9" t="str">
+      <c r="R4" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Representante SA</v>
       </c>
-      <c r="R4" s="9" t="str">
+      <c r="S4" s="9" t="str">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="S4" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R4,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T4" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R4,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S4,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U4" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S4,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -919,55 +901,58 @@
       <c r="H5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="12" t="str">
+      <c r="I5" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J5" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J5" s="12" t="str">
+      <c r="K5" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K5" s="11">
+      <c r="L5" s="11">
         <v>44896</v>
       </c>
-      <c r="L5" s="9" t="str">
+      <c r="M5" s="9" t="str">
         <f t="shared" si="5"/>
         <v>12/2022</v>
       </c>
-      <c r="M5" s="9">
+      <c r="N5" s="9">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="N5" s="9">
+      <c r="O5" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q5" s="9" t="str">
+      <c r="R5" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202212 - Cliente 2</v>
       </c>
-      <c r="R5" s="9" t="str">
+      <c r="S5" s="9" t="str">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="S5" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R5,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T5" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R5,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S5,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U5" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S5,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -987,55 +972,58 @@
       <c r="H6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="12" t="str">
-        <f t="shared" ref="I6" si="10">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;M6&amp;"\"&amp;TEXT(N6,"00")&amp;"\"</f>
+      <c r="I6" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J6" s="12" t="str">
+        <f t="shared" ref="J6" si="10">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;N6&amp;"\"&amp;TEXT(O6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2007\01\</v>
       </c>
-      <c r="J6" s="12" t="str">
-        <f t="shared" ref="J6" si="11">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;M6&amp;"\"&amp;TEXT(N6,"00")&amp;"\"</f>
+      <c r="K6" s="12" t="str">
+        <f t="shared" ref="K6" si="11">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;N6&amp;"\"&amp;TEXT(O6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2007\01\</v>
       </c>
-      <c r="K6" s="11">
+      <c r="L6" s="11">
         <v>39083</v>
       </c>
-      <c r="L6" s="9" t="str">
+      <c r="M6" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2007</v>
       </c>
-      <c r="M6" s="9">
-        <f t="shared" ref="M6" si="12">YEAR(K6)</f>
+      <c r="N6" s="9">
+        <f t="shared" ref="N6" si="12">YEAR(L6)</f>
         <v>2007</v>
       </c>
-      <c r="N6" s="9">
-        <f t="shared" ref="N6" si="13">MONTH(K6)</f>
+      <c r="O6" s="9">
+        <f t="shared" ref="O6" si="13">MONTH(L6)</f>
         <v>1</v>
       </c>
-      <c r="O6" s="9">
+      <c r="P6" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P6" s="9">
+      <c r="Q6" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q6" s="9" t="str">
-        <f t="shared" ref="Q6" si="14">CONCATENATE(B6," - ",TEXT(K6,"AAAAMM")," - ",IF(F6="",A6,F6))</f>
+      <c r="R6" s="9" t="str">
+        <f t="shared" ref="R6" si="14">CONCATENATE(B6," - ",TEXT(L6,"AAAAMM")," - ",IF(F6="",A6,F6))</f>
         <v>20000000000 - 200701 - Cliente 2</v>
       </c>
-      <c r="R6" s="9" t="str">
-        <f t="shared" ref="R6" si="15">TEXT(ROW(A6),"0")</f>
+      <c r="S6" s="9" t="str">
+        <f t="shared" ref="S6" si="15">TEXT(ROW(A6),"0")</f>
         <v>6</v>
       </c>
-      <c r="S6" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R6,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T6" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R6,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S6,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U6" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S6,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1055,55 +1043,58 @@
       <c r="H7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="12" t="str">
+      <c r="I7" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J7" s="12" t="str">
+      <c r="K7" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K7" s="11">
+      <c r="L7" s="11">
         <v>44927</v>
       </c>
-      <c r="L7" s="9" t="str">
+      <c r="M7" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2023</v>
       </c>
-      <c r="M7" s="9">
+      <c r="N7" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="N7" s="9">
+      <c r="O7" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O7" s="9">
+      <c r="P7" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P7" s="9">
+      <c r="Q7" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q7" s="9" t="str">
+      <c r="R7" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202301 - Cliente 2</v>
       </c>
-      <c r="R7" s="9" t="str">
+      <c r="S7" s="9" t="str">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="S7" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R7,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T7" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R7,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S7,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U7" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S7,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1123,55 +1114,58 @@
       <c r="H8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="12" t="str">
+      <c r="I8" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J8" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J8" s="12" t="str">
+      <c r="K8" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K8" s="11">
+      <c r="L8" s="11">
         <v>44958</v>
       </c>
-      <c r="L8" s="9" t="str">
+      <c r="M8" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="M8" s="9">
+      <c r="N8" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="N8" s="9">
+      <c r="O8" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O8" s="9">
+      <c r="P8" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="9" t="str">
+      <c r="R8" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Cliente 2</v>
       </c>
-      <c r="R8" s="9" t="str">
+      <c r="S8" s="9" t="str">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="S8" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R8,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T8" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R8,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S8,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U8" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S8,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1191,55 +1185,58 @@
       <c r="H9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="12" t="str">
+      <c r="I9" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J9" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J9" s="12" t="str">
+      <c r="K9" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K9" s="11">
+      <c r="L9" s="11">
         <v>44896</v>
       </c>
-      <c r="L9" s="9" t="str">
+      <c r="M9" s="9" t="str">
         <f t="shared" si="5"/>
         <v>12/2022</v>
       </c>
-      <c r="M9" s="9">
+      <c r="N9" s="9">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="N9" s="9">
+      <c r="O9" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="O9" s="9">
+      <c r="P9" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q9" s="9" t="str">
+      <c r="R9" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202212 - Cliente 3</v>
       </c>
-      <c r="R9" s="9" t="str">
+      <c r="S9" s="9" t="str">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="S9" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R9,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T9" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R9,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S9,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U9" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S9,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1259,55 +1256,58 @@
       <c r="H10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="12" t="str">
+      <c r="I10" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J10" s="12" t="str">
+      <c r="K10" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K10" s="11">
+      <c r="L10" s="11">
         <v>44927</v>
       </c>
-      <c r="L10" s="9" t="str">
+      <c r="M10" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2023</v>
       </c>
-      <c r="M10" s="9">
+      <c r="N10" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="N10" s="9">
+      <c r="O10" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="O10" s="9">
+      <c r="P10" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q10" s="9" t="str">
+      <c r="R10" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202301 - Cliente 3</v>
       </c>
-      <c r="R10" s="9" t="str">
+      <c r="S10" s="9" t="str">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="S10" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R10,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T10" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R10,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S10,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U10" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S10,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1327,55 +1327,58 @@
       <c r="H11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="12" t="str">
+      <c r="I11" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J11" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J11" s="12" t="str">
+      <c r="K11" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K11" s="11">
+      <c r="L11" s="11">
         <v>44958</v>
       </c>
-      <c r="L11" s="9" t="str">
+      <c r="M11" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="M11" s="9">
+      <c r="N11" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="N11" s="9">
+      <c r="O11" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="O11" s="9">
+      <c r="P11" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q11" s="9" t="str">
+      <c r="R11" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Cliente 3</v>
       </c>
-      <c r="R11" s="9" t="str">
+      <c r="S11" s="9" t="str">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="S11" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R11,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T11" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R11,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S11,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U11" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S11,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1395,55 +1398,58 @@
       <c r="H12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="12" t="str">
+      <c r="I12" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="J12" s="12" t="str">
+      <c r="K12" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="K12" s="11">
+      <c r="L12" s="11">
         <v>44896</v>
       </c>
-      <c r="L12" s="9" t="str">
+      <c r="M12" s="9" t="str">
         <f t="shared" si="5"/>
         <v>12/2022</v>
       </c>
-      <c r="M12" s="9">
-        <f t="shared" ref="M12:M14" si="16">YEAR(K12)</f>
+      <c r="N12" s="9">
+        <f t="shared" ref="N12:N14" si="16">YEAR(L12)</f>
         <v>2022</v>
       </c>
-      <c r="N12" s="9">
-        <f t="shared" ref="N12:N14" si="17">MONTH(K12)</f>
+      <c r="O12" s="9">
+        <f t="shared" ref="O12:O14" si="17">MONTH(L12)</f>
         <v>12</v>
       </c>
-      <c r="O12" s="9">
+      <c r="P12" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P12" s="9">
+      <c r="Q12" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q12" s="9" t="str">
+      <c r="R12" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202212 - Cliente 4</v>
       </c>
-      <c r="R12" s="9" t="str">
+      <c r="S12" s="9" t="str">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="S12" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R12,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T12" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R12,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S12,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U12" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S12,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1463,55 +1469,58 @@
       <c r="H13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="12" t="str">
+      <c r="I13" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="J13" s="12" t="str">
+      <c r="K13" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="K13" s="11">
+      <c r="L13" s="11">
         <v>44927</v>
       </c>
-      <c r="L13" s="9" t="str">
+      <c r="M13" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2023</v>
       </c>
-      <c r="M13" s="9">
+      <c r="N13" s="9">
         <f t="shared" si="16"/>
         <v>2023</v>
       </c>
-      <c r="N13" s="9">
+      <c r="O13" s="9">
         <f t="shared" si="17"/>
         <v>1</v>
       </c>
-      <c r="O13" s="9">
+      <c r="P13" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P13" s="9">
+      <c r="Q13" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="Q13" s="9" t="str">
+      <c r="R13" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202301 - Cliente 4</v>
       </c>
-      <c r="R13" s="9" t="str">
+      <c r="S13" s="9" t="str">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="S13" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R13,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T13" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R13,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S13,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U13" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S13,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1531,59 +1540,67 @@
       <c r="H14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="12" t="str">
+      <c r="I14" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="J14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="J14" s="12" t="str">
+      <c r="K14" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="K14" s="11">
+      <c r="L14" s="11">
         <v>44958</v>
       </c>
-      <c r="L14" s="9" t="str">
+      <c r="M14" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="M14" s="9">
+      <c r="N14" s="9">
         <f t="shared" si="16"/>
         <v>2023</v>
       </c>
-      <c r="N14" s="9">
+      <c r="O14" s="9">
         <f t="shared" si="17"/>
         <v>2</v>
       </c>
-      <c r="O14" s="9">
+      <c r="P14" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="P14" s="9">
+      <c r="Q14" s="9">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="Q14" s="9" t="str">
+      <c r="R14" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Cliente 4</v>
       </c>
-      <c r="R14" s="9" t="str">
+      <c r="S14" s="9" t="str">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="S14" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R14,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="T14" s="9" t="str">
-        <f>IFERROR(VLOOKUP(R14,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(S14,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="U14" s="9" t="str">
+        <f>IFERROR(VLOOKUP(S14,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:T14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:U14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4">
     <sortCondition ref="A2"/>
   </sortState>
+  <dataValidations count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:I14" xr:uid="{16927795-E0AC-4AAA-87BF-385CFC41B068}">
+      <formula1>"SI,NO"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>

<commit_message>
Edit Excel to match all regions
</commit_message>
<xml_diff>
--- a/RETPER ARBA AGIP.xlsx
+++ b/RETPER ARBA AGIP.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\RETPER-IIBB-AGIP-ARBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DEDC84C-75B5-43E5-A4F2-16F15609A11C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAE93AC-A5FF-49B2-9786-F030A557C3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -711,7 +711,7 @@
         <v>44896</v>
       </c>
       <c r="N2" s="9" t="str">
-        <f>TEXT(M2,"MM/AAAA")</f>
+        <f>TEXT(P2,"00")&amp;"/"&amp;O2</f>
         <v>12/2022</v>
       </c>
       <c r="O2" s="9">
@@ -731,7 +731,7 @@
         <v>0</v>
       </c>
       <c r="S2" s="9" t="str">
-        <f>CONCATENATE(B2," - ",TEXT(M2,"AAAAMM")," - ",IF(F2="",A2,F2))</f>
+        <f>CONCATENATE(B2," - ",O2,TEXT(P2,"00")," - ",IF(F2="",A2,F2))</f>
         <v>20000000000 - 202212 - Representante SA</v>
       </c>
       <c r="T2" s="9" t="str">
@@ -787,7 +787,7 @@
         <v>44927</v>
       </c>
       <c r="N3" s="9" t="str">
-        <f t="shared" ref="N3:N14" si="5">TEXT(M3,"MM/AAAA")</f>
+        <f t="shared" ref="N3:N14" si="5">TEXT(P3,"00")&amp;"/"&amp;O3</f>
         <v>01/2023</v>
       </c>
       <c r="O3" s="9">
@@ -807,7 +807,7 @@
         <v>0</v>
       </c>
       <c r="S3" s="9" t="str">
-        <f t="shared" ref="S3:S14" si="8">CONCATENATE(B3," - ",TEXT(M3,"AAAAMM")," - ",IF(F3="",A3,F3))</f>
+        <f t="shared" ref="S3:S14" si="8">CONCATENATE(B3," - ",O3,TEXT(P3,"00")," - ",IF(F3="",A3,F3))</f>
         <v>20000000000 - 202301 - Representante SA</v>
       </c>
       <c r="T3" s="9" t="str">
@@ -1031,11 +1031,11 @@
         <v>0</v>
       </c>
       <c r="S6" s="9" t="str">
-        <f t="shared" ref="S6" si="14">CONCATENATE(B6," - ",TEXT(M6,"AAAAMM")," - ",IF(F6="",A6,F6))</f>
+        <f t="shared" si="8"/>
         <v>20000000000 - 200701 - Cliente 2</v>
       </c>
       <c r="T6" s="9" t="str">
-        <f t="shared" ref="T6" si="15">TEXT(ROW(A6),"0")</f>
+        <f t="shared" ref="T6" si="14">TEXT(ROW(A6),"0")</f>
         <v>6</v>
       </c>
       <c r="U6" s="9" t="str">
@@ -1459,11 +1459,11 @@
         <v>12/2022</v>
       </c>
       <c r="O12" s="9">
-        <f t="shared" ref="O12:O14" si="16">YEAR(M12)</f>
+        <f t="shared" ref="O12:O14" si="15">YEAR(M12)</f>
         <v>2022</v>
       </c>
       <c r="P12" s="9">
-        <f t="shared" ref="P12:P14" si="17">MONTH(M12)</f>
+        <f t="shared" ref="P12:P14" si="16">MONTH(M12)</f>
         <v>12</v>
       </c>
       <c r="Q12" s="9">
@@ -1533,11 +1533,11 @@
         <v>01/2023</v>
       </c>
       <c r="O13" s="9">
+        <f t="shared" si="15"/>
+        <v>2023</v>
+      </c>
+      <c r="P13" s="9">
         <f t="shared" si="16"/>
-        <v>2023</v>
-      </c>
-      <c r="P13" s="9">
-        <f t="shared" si="17"/>
         <v>1</v>
       </c>
       <c r="Q13" s="9">
@@ -1607,11 +1607,11 @@
         <v>02/2023</v>
       </c>
       <c r="O14" s="9">
+        <f t="shared" si="15"/>
+        <v>2023</v>
+      </c>
+      <c r="P14" s="9">
         <f t="shared" si="16"/>
-        <v>2023</v>
-      </c>
-      <c r="P14" s="9">
-        <f t="shared" si="17"/>
         <v>2</v>
       </c>
       <c r="Q14" s="9">

</xml_diff>

<commit_message>
Add CUIT ARBA Column
</commit_message>
<xml_diff>
--- a/RETPER ARBA AGIP.xlsx
+++ b/RETPER ARBA AGIP.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Proyectos Uipath\RETPER-IIBB-AGIP-ARBA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AAE93AC-A5FF-49B2-9786-F030A557C3B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D23F1D7-7B9E-4FE4-BB24-04C236914E0A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
     <externalReference r:id="rId2"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$V$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Clientes!$A$1:$W$14</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="32">
   <si>
     <t>CLIENTES</t>
   </si>
@@ -132,6 +132,9 @@
   </si>
   <si>
     <t>NO</t>
+  </si>
+  <si>
+    <t>CUIT ARBA</t>
   </si>
 </sst>
 </file>
@@ -585,25 +588,28 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V14"/>
+  <dimension ref="A1:W14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.5703125" style="1" customWidth="1"/>
     <col min="2" max="2" width="23.140625" style="1" customWidth="1"/>
     <col min="3" max="3" width="21.28515625" style="1" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="17.28515625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
-    <col min="6" max="7" width="25.85546875" style="1" customWidth="1"/>
-    <col min="8" max="12" width="19.7109375" style="1" customWidth="1"/>
-    <col min="13" max="13" width="13" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="11.42578125" style="1"/>
+    <col min="4" max="4" width="21.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="17.28515625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" style="1" customWidth="1"/>
+    <col min="7" max="8" width="25.85546875" style="1" customWidth="1"/>
+    <col min="9" max="13" width="19.7109375" style="1" customWidth="1"/>
+    <col min="14" max="14" width="13" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -614,64 +620,67 @@
         <v>2</v>
       </c>
       <c r="D1" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="8" t="s">
+      <c r="G1" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="8" t="s">
+      <c r="H1" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="I1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="I1" s="8" t="s">
+      <c r="J1" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="J1" s="8" t="s">
+      <c r="K1" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="L1" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="8" t="s">
+      <c r="M1" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="N1" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="8" t="s">
+      <c r="O1" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="O1" s="8" t="s">
+      <c r="P1" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="P1" s="8" t="s">
+      <c r="Q1" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="R1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="R1" s="8" t="s">
+      <c r="S1" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="S1" s="8" t="s">
+      <c r="T1" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="T1" s="8" t="s">
+      <c r="U1" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="U1" s="8" t="s">
+      <c r="V1" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="V1" s="8" t="s">
+      <c r="W1" s="8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>21</v>
       </c>
@@ -679,75 +688,78 @@
         <v>20000000000</v>
       </c>
       <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G2" s="7" t="str">
-        <f>IF(F2="","",CONCATENATE(UPPER(F2)))</f>
+      <c r="H2" s="7" t="str">
+        <f>IF(G2="","",CONCATENATE(UPPER(G2)))</f>
         <v>REPRESENTANTE SA</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="I2" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="J2" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="K2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K2" s="12" t="str">
-        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\ARBA\"&amp;O2&amp;"\"&amp;TEXT(P2,"00")&amp;"\"</f>
+      <c r="L2" s="12" t="str">
+        <f>I2&amp;"\"&amp;IF(G2="",A2,G2)&amp;"\RETPER\ARBA\"&amp;P2&amp;"\"&amp;TEXT(Q2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="L2" s="12" t="str">
-        <f>H2&amp;"\"&amp;IF(F2="",A2,F2)&amp;"\RETPER\AGIP\"&amp;O2&amp;"\"&amp;TEXT(P2,"00")&amp;"\"</f>
+      <c r="M2" s="12" t="str">
+        <f>I2&amp;"\"&amp;IF(G2="",A2,G2)&amp;"\RETPER\AGIP\"&amp;P2&amp;"\"&amp;TEXT(Q2,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="M2" s="11">
+      <c r="N2" s="11">
         <v>44896</v>
       </c>
-      <c r="N2" s="9" t="str">
-        <f>TEXT(P2,"00")&amp;"/"&amp;O2</f>
+      <c r="O2" s="9" t="str">
+        <f>TEXT(Q2,"00")&amp;"/"&amp;P2</f>
         <v>12/2022</v>
       </c>
-      <c r="O2" s="9">
-        <f t="shared" ref="O2:O11" si="0">YEAR(M2)</f>
+      <c r="P2" s="9">
+        <f t="shared" ref="P2:P11" si="0">YEAR(N2)</f>
         <v>2022</v>
       </c>
-      <c r="P2" s="9">
-        <f t="shared" ref="P2:P11" si="1">MONTH(M2)</f>
+      <c r="Q2" s="9">
+        <f t="shared" ref="Q2:Q11" si="1">MONTH(N2)</f>
         <v>12</v>
       </c>
-      <c r="Q2" s="9">
+      <c r="R2" s="9">
         <f>IF(B2=B1,0,1)</f>
         <v>1</v>
       </c>
-      <c r="R2" s="9">
+      <c r="S2" s="9">
         <f>IF(B3=B2,0,1)</f>
         <v>0</v>
       </c>
-      <c r="S2" s="9" t="str">
-        <f>CONCATENATE(B2," - ",O2,TEXT(P2,"00")," - ",IF(F2="",A2,F2))</f>
+      <c r="T2" s="9" t="str">
+        <f>CONCATENATE(B2," - ",P2,TEXT(Q2,"00")," - ",IF(G2="",A2,G2))</f>
         <v>20000000000 - 202212 - Representante SA</v>
       </c>
-      <c r="T2" s="9" t="str">
+      <c r="U2" s="9" t="str">
         <f>TEXT(ROW(A2),"0")</f>
         <v>2</v>
       </c>
-      <c r="U2" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T2,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V2" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T2,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U2,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W2" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U2,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
@@ -755,75 +767,78 @@
         <v>20000000000</v>
       </c>
       <c r="C3" s="6"/>
-      <c r="D3" s="6"/>
-      <c r="E3" s="4" t="s">
+      <c r="D3" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E3" s="6"/>
+      <c r="F3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="7" t="s">
+      <c r="G3" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G3" s="7" t="str">
-        <f t="shared" ref="G3:G14" si="2">IF(F3="","",CONCATENATE(UPPER(F3)))</f>
+      <c r="H3" s="7" t="str">
+        <f t="shared" ref="H3:H14" si="2">IF(G3="","",CONCATENATE(UPPER(G3)))</f>
         <v>REPRESENTANTE SA</v>
       </c>
-      <c r="H3" s="10" t="s">
+      <c r="I3" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="10" t="s">
+      <c r="J3" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="10" t="s">
+      <c r="K3" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K3" s="12" t="str">
-        <f t="shared" ref="K3:K14" si="3">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\ARBA\"&amp;O3&amp;"\"&amp;TEXT(P3,"00")&amp;"\"</f>
+      <c r="L3" s="12" t="str">
+        <f t="shared" ref="L3:L14" si="3">I3&amp;"\"&amp;IF(G3="",A3,G3)&amp;"\RETPER\ARBA\"&amp;P3&amp;"\"&amp;TEXT(Q3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="L3" s="12" t="str">
-        <f t="shared" ref="L3:L14" si="4">H3&amp;"\"&amp;IF(F3="",A3,F3)&amp;"\RETPER\AGIP\"&amp;O3&amp;"\"&amp;TEXT(P3,"00")&amp;"\"</f>
+      <c r="M3" s="12" t="str">
+        <f t="shared" ref="M3:M14" si="4">I3&amp;"\"&amp;IF(G3="",A3,G3)&amp;"\RETPER\AGIP\"&amp;P3&amp;"\"&amp;TEXT(Q3,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="M3" s="11">
+      <c r="N3" s="11">
         <v>44927</v>
       </c>
-      <c r="N3" s="9" t="str">
-        <f t="shared" ref="N3:N14" si="5">TEXT(P3,"00")&amp;"/"&amp;O3</f>
+      <c r="O3" s="9" t="str">
+        <f t="shared" ref="O3:O14" si="5">TEXT(Q3,"00")&amp;"/"&amp;P3</f>
         <v>01/2023</v>
       </c>
-      <c r="O3" s="9">
+      <c r="P3" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="P3" s="9">
+      <c r="Q3" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q3" s="9">
-        <f t="shared" ref="Q3:Q14" si="6">IF(B3=B2,0,1)</f>
-        <v>0</v>
-      </c>
       <c r="R3" s="9">
-        <f t="shared" ref="R3:R14" si="7">IF(B4=B3,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="S3" s="9" t="str">
-        <f t="shared" ref="S3:S14" si="8">CONCATENATE(B3," - ",O3,TEXT(P3,"00")," - ",IF(F3="",A3,F3))</f>
+        <f t="shared" ref="R3:R14" si="6">IF(B3=B2,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="S3" s="9">
+        <f t="shared" ref="S3:S14" si="7">IF(B4=B3,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="9" t="str">
+        <f t="shared" ref="T3:T14" si="8">CONCATENATE(B3," - ",P3,TEXT(Q3,"00")," - ",IF(G3="",A3,G3))</f>
         <v>20000000000 - 202301 - Representante SA</v>
       </c>
-      <c r="T3" s="9" t="str">
-        <f t="shared" ref="T3:T14" si="9">TEXT(ROW(A3),"0")</f>
+      <c r="U3" s="9" t="str">
+        <f t="shared" ref="U3:U14" si="9">TEXT(ROW(A3),"0")</f>
         <v>3</v>
       </c>
-      <c r="U3" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T3,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V3" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T3,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U3,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W3" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U3,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>21</v>
       </c>
@@ -831,75 +846,78 @@
         <v>20000000000</v>
       </c>
       <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="4" t="s">
+      <c r="D4" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E4" s="6"/>
+      <c r="F4" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="G4" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="G4" s="7" t="str">
+      <c r="H4" s="7" t="str">
         <f t="shared" si="2"/>
         <v>REPRESENTANTE SA</v>
       </c>
-      <c r="H4" s="10" t="s">
+      <c r="I4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I4" s="10" t="s">
+      <c r="J4" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J4" s="10" t="s">
+      <c r="K4" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K4" s="12" t="str">
+      <c r="L4" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="L4" s="12" t="str">
+      <c r="M4" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Representante SA\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="M4" s="11">
+      <c r="N4" s="11">
         <v>44958</v>
       </c>
-      <c r="N4" s="9" t="str">
+      <c r="O4" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="O4" s="9">
+      <c r="P4" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="P4" s="9">
+      <c r="Q4" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q4" s="9">
+      <c r="R4" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R4" s="9">
+      <c r="S4" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S4" s="9" t="str">
+      <c r="T4" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Representante SA</v>
       </c>
-      <c r="T4" s="9" t="str">
+      <c r="U4" s="9" t="str">
         <f t="shared" si="9"/>
         <v>4</v>
       </c>
-      <c r="U4" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T4,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V4" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T4,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U4,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W4" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U4,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
@@ -907,73 +925,76 @@
         <v>20000000000</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="5">
+        <v>20000000000</v>
+      </c>
+      <c r="E5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E5" s="4"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="7" t="str">
+      <c r="F5" s="4"/>
+      <c r="G5" s="2"/>
+      <c r="H5" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="I5" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="10" t="s">
+      <c r="J5" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J5" s="10" t="s">
+      <c r="K5" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K5" s="12" t="str">
+      <c r="L5" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="L5" s="12" t="str">
+      <c r="M5" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="M5" s="11">
+      <c r="N5" s="11">
         <v>44896</v>
       </c>
-      <c r="N5" s="9" t="str">
+      <c r="O5" s="9" t="str">
         <f t="shared" si="5"/>
         <v>12/2022</v>
       </c>
-      <c r="O5" s="9">
+      <c r="P5" s="9">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="P5" s="9">
+      <c r="Q5" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="Q5" s="9">
+      <c r="R5" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R5" s="9">
+      <c r="S5" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S5" s="9" t="str">
+      <c r="T5" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202212 - Cliente 2</v>
       </c>
-      <c r="T5" s="9" t="str">
+      <c r="U5" s="9" t="str">
         <f t="shared" si="9"/>
         <v>5</v>
       </c>
-      <c r="U5" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T5,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V5" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T5,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U5,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W5" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U5,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>22</v>
       </c>
@@ -981,73 +1002,76 @@
         <v>20000000000</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="4" t="s">
+      <c r="D6" s="5">
+        <v>20000000000</v>
+      </c>
+      <c r="E6" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E6" s="4"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="7" t="str">
+      <c r="F6" s="4"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H6" s="10" t="s">
+      <c r="I6" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="10" t="s">
+      <c r="J6" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J6" s="10" t="s">
+      <c r="K6" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K6" s="12" t="str">
-        <f t="shared" ref="K6" si="10">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\ARBA\"&amp;O6&amp;"\"&amp;TEXT(P6,"00")&amp;"\"</f>
+      <c r="L6" s="12" t="str">
+        <f t="shared" ref="L6" si="10">I6&amp;"\"&amp;IF(G6="",A6,G6)&amp;"\RETPER\ARBA\"&amp;P6&amp;"\"&amp;TEXT(Q6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2007\01\</v>
       </c>
-      <c r="L6" s="12" t="str">
-        <f t="shared" ref="L6" si="11">H6&amp;"\"&amp;IF(F6="",A6,F6)&amp;"\RETPER\AGIP\"&amp;O6&amp;"\"&amp;TEXT(P6,"00")&amp;"\"</f>
+      <c r="M6" s="12" t="str">
+        <f t="shared" ref="M6" si="11">I6&amp;"\"&amp;IF(G6="",A6,G6)&amp;"\RETPER\AGIP\"&amp;P6&amp;"\"&amp;TEXT(Q6,"00")&amp;"\"</f>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2007\01\</v>
       </c>
-      <c r="M6" s="11">
+      <c r="N6" s="11">
         <v>39083</v>
       </c>
-      <c r="N6" s="9" t="str">
+      <c r="O6" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2007</v>
       </c>
-      <c r="O6" s="9">
-        <f t="shared" ref="O6" si="12">YEAR(M6)</f>
+      <c r="P6" s="9">
+        <f t="shared" ref="P6" si="12">YEAR(N6)</f>
         <v>2007</v>
       </c>
-      <c r="P6" s="9">
-        <f t="shared" ref="P6" si="13">MONTH(M6)</f>
+      <c r="Q6" s="9">
+        <f t="shared" ref="Q6" si="13">MONTH(N6)</f>
         <v>1</v>
       </c>
-      <c r="Q6" s="9">
+      <c r="R6" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R6" s="9">
+      <c r="S6" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S6" s="9" t="str">
+      <c r="T6" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 200701 - Cliente 2</v>
       </c>
-      <c r="T6" s="9" t="str">
-        <f t="shared" ref="T6" si="14">TEXT(ROW(A6),"0")</f>
+      <c r="U6" s="9" t="str">
+        <f t="shared" ref="U6" si="14">TEXT(ROW(A6),"0")</f>
         <v>6</v>
       </c>
-      <c r="U6" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T6,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V6" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T6,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U6,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W6" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U6,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="7" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>22</v>
       </c>
@@ -1055,73 +1079,76 @@
         <v>20000000000</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="4" t="s">
+      <c r="D7" s="5">
+        <v>20000000000</v>
+      </c>
+      <c r="E7" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E7" s="4"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="7" t="str">
+      <c r="F7" s="4"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H7" s="10" t="s">
+      <c r="I7" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="10" t="s">
+      <c r="J7" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J7" s="10" t="s">
+      <c r="K7" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K7" s="12" t="str">
+      <c r="L7" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="L7" s="12" t="str">
+      <c r="M7" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="M7" s="11">
+      <c r="N7" s="11">
         <v>44927</v>
       </c>
-      <c r="N7" s="9" t="str">
+      <c r="O7" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2023</v>
       </c>
-      <c r="O7" s="9">
+      <c r="P7" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="P7" s="9">
+      <c r="Q7" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q7" s="9">
+      <c r="R7" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R7" s="9">
+      <c r="S7" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S7" s="9" t="str">
+      <c r="T7" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202301 - Cliente 2</v>
       </c>
-      <c r="T7" s="9" t="str">
+      <c r="U7" s="9" t="str">
         <f t="shared" si="9"/>
         <v>7</v>
       </c>
-      <c r="U7" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T7,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V7" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T7,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U7,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W7" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U7,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>22</v>
       </c>
@@ -1129,73 +1156,76 @@
         <v>20000000000</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="4" t="s">
+      <c r="D8" s="5">
+        <v>20000000000</v>
+      </c>
+      <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="E8" s="4"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="7" t="str">
+      <c r="F8" s="4"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H8" s="10" t="s">
+      <c r="I8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I8" s="10" t="s">
+      <c r="J8" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J8" s="10" t="s">
+      <c r="K8" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K8" s="12" t="str">
+      <c r="L8" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="L8" s="12" t="str">
+      <c r="M8" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 2\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="M8" s="11">
+      <c r="N8" s="11">
         <v>44958</v>
       </c>
-      <c r="N8" s="9" t="str">
+      <c r="O8" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="O8" s="9">
+      <c r="P8" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="P8" s="9">
+      <c r="Q8" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q8" s="9">
+      <c r="R8" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R8" s="9">
+      <c r="S8" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S8" s="9" t="str">
+      <c r="T8" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Cliente 2</v>
       </c>
-      <c r="T8" s="9" t="str">
+      <c r="U8" s="9" t="str">
         <f t="shared" si="9"/>
         <v>8</v>
       </c>
-      <c r="U8" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T8,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V8" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T8,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U8,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W8" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U8,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>23</v>
       </c>
@@ -1203,73 +1233,76 @@
         <v>20000000000</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4" t="s">
+      <c r="D9" s="5">
+        <v>20000000000</v>
+      </c>
+      <c r="E9" s="4"/>
+      <c r="F9" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F9" s="2"/>
-      <c r="G9" s="7" t="str">
+      <c r="G9" s="2"/>
+      <c r="H9" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H9" s="10" t="s">
+      <c r="I9" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I9" s="10" t="s">
+      <c r="J9" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J9" s="10" t="s">
+      <c r="K9" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K9" s="12" t="str">
+      <c r="L9" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="L9" s="12" t="str">
+      <c r="M9" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="M9" s="11">
+      <c r="N9" s="11">
         <v>44896</v>
       </c>
-      <c r="N9" s="9" t="str">
+      <c r="O9" s="9" t="str">
         <f t="shared" si="5"/>
         <v>12/2022</v>
       </c>
-      <c r="O9" s="9">
+      <c r="P9" s="9">
         <f t="shared" si="0"/>
         <v>2022</v>
       </c>
-      <c r="P9" s="9">
+      <c r="Q9" s="9">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="Q9" s="9">
+      <c r="R9" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R9" s="9">
+      <c r="S9" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S9" s="9" t="str">
+      <c r="T9" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202212 - Cliente 3</v>
       </c>
-      <c r="T9" s="9" t="str">
+      <c r="U9" s="9" t="str">
         <f t="shared" si="9"/>
         <v>9</v>
       </c>
-      <c r="U9" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T9,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V9" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T9,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U9,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W9" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U9,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>23</v>
       </c>
@@ -1277,73 +1310,76 @@
         <v>20000000000</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4" t="s">
+      <c r="D10" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F10" s="2"/>
-      <c r="G10" s="7" t="str">
+      <c r="G10" s="2"/>
+      <c r="H10" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H10" s="10" t="s">
+      <c r="I10" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I10" s="10" t="s">
+      <c r="J10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J10" s="10" t="s">
+      <c r="K10" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K10" s="12" t="str">
+      <c r="L10" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="L10" s="12" t="str">
+      <c r="M10" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="M10" s="11">
+      <c r="N10" s="11">
         <v>44927</v>
       </c>
-      <c r="N10" s="9" t="str">
+      <c r="O10" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2023</v>
       </c>
-      <c r="O10" s="9">
+      <c r="P10" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="P10" s="9">
+      <c r="Q10" s="9">
         <f t="shared" si="1"/>
         <v>1</v>
       </c>
-      <c r="Q10" s="9">
+      <c r="R10" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R10" s="9">
+      <c r="S10" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S10" s="9" t="str">
+      <c r="T10" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202301 - Cliente 3</v>
       </c>
-      <c r="T10" s="9" t="str">
+      <c r="U10" s="9" t="str">
         <f t="shared" si="9"/>
         <v>10</v>
       </c>
-      <c r="U10" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T10,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V10" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T10,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U10,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W10" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U10,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="11" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>23</v>
       </c>
@@ -1351,73 +1387,76 @@
         <v>20000000000</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4" t="s">
+      <c r="D11" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F11" s="2"/>
-      <c r="G11" s="7" t="str">
+      <c r="G11" s="2"/>
+      <c r="H11" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H11" s="10" t="s">
+      <c r="I11" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I11" s="10" t="s">
+      <c r="J11" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J11" s="10" t="s">
+      <c r="K11" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K11" s="12" t="str">
+      <c r="L11" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="L11" s="12" t="str">
+      <c r="M11" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 3\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="M11" s="11">
+      <c r="N11" s="11">
         <v>44958</v>
       </c>
-      <c r="N11" s="9" t="str">
+      <c r="O11" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="O11" s="9">
+      <c r="P11" s="9">
         <f t="shared" si="0"/>
         <v>2023</v>
       </c>
-      <c r="P11" s="9">
+      <c r="Q11" s="9">
         <f t="shared" si="1"/>
         <v>2</v>
       </c>
-      <c r="Q11" s="9">
+      <c r="R11" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R11" s="9">
+      <c r="S11" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S11" s="9" t="str">
+      <c r="T11" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Cliente 3</v>
       </c>
-      <c r="T11" s="9" t="str">
+      <c r="U11" s="9" t="str">
         <f t="shared" si="9"/>
         <v>11</v>
       </c>
-      <c r="U11" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T11,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V11" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T11,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U11,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W11" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U11,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>24</v>
       </c>
@@ -1425,73 +1464,76 @@
         <v>20000000000</v>
       </c>
       <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="4" t="s">
+      <c r="D12" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="7" t="str">
+      <c r="G12" s="2"/>
+      <c r="H12" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H12" s="10" t="s">
+      <c r="I12" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I12" s="10" t="s">
+      <c r="J12" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J12" s="10" t="s">
+      <c r="K12" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="12" t="str">
+      <c r="L12" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\ARBA\2022\12\</v>
       </c>
-      <c r="L12" s="12" t="str">
+      <c r="M12" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\AGIP\2022\12\</v>
       </c>
-      <c r="M12" s="11">
+      <c r="N12" s="11">
         <v>44896</v>
       </c>
-      <c r="N12" s="9" t="str">
+      <c r="O12" s="9" t="str">
         <f t="shared" si="5"/>
         <v>12/2022</v>
       </c>
-      <c r="O12" s="9">
-        <f t="shared" ref="O12:O14" si="15">YEAR(M12)</f>
+      <c r="P12" s="9">
+        <f t="shared" ref="P12:P14" si="15">YEAR(N12)</f>
         <v>2022</v>
       </c>
-      <c r="P12" s="9">
-        <f t="shared" ref="P12:P14" si="16">MONTH(M12)</f>
+      <c r="Q12" s="9">
+        <f t="shared" ref="Q12:Q14" si="16">MONTH(N12)</f>
         <v>12</v>
       </c>
-      <c r="Q12" s="9">
+      <c r="R12" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R12" s="9">
+      <c r="S12" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S12" s="9" t="str">
+      <c r="T12" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202212 - Cliente 4</v>
       </c>
-      <c r="T12" s="9" t="str">
+      <c r="U12" s="9" t="str">
         <f t="shared" si="9"/>
         <v>12</v>
       </c>
-      <c r="U12" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T12,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V12" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T12,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U12,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W12" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U12,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="13" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>24</v>
       </c>
@@ -1499,73 +1541,76 @@
         <v>20000000000</v>
       </c>
       <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="4" t="s">
+      <c r="D13" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E13" s="2"/>
+      <c r="F13" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="7" t="str">
+      <c r="G13" s="2"/>
+      <c r="H13" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H13" s="10" t="s">
+      <c r="I13" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I13" s="10" t="s">
+      <c r="J13" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J13" s="10" t="s">
+      <c r="K13" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K13" s="12" t="str">
+      <c r="L13" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\ARBA\2023\01\</v>
       </c>
-      <c r="L13" s="12" t="str">
+      <c r="M13" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\AGIP\2023\01\</v>
       </c>
-      <c r="M13" s="11">
+      <c r="N13" s="11">
         <v>44927</v>
       </c>
-      <c r="N13" s="9" t="str">
+      <c r="O13" s="9" t="str">
         <f t="shared" si="5"/>
         <v>01/2023</v>
       </c>
-      <c r="O13" s="9">
+      <c r="P13" s="9">
         <f t="shared" si="15"/>
         <v>2023</v>
       </c>
-      <c r="P13" s="9">
+      <c r="Q13" s="9">
         <f t="shared" si="16"/>
         <v>1</v>
       </c>
-      <c r="Q13" s="9">
+      <c r="R13" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R13" s="9">
+      <c r="S13" s="9">
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-      <c r="S13" s="9" t="str">
+      <c r="T13" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202301 - Cliente 4</v>
       </c>
-      <c r="T13" s="9" t="str">
+      <c r="U13" s="9" t="str">
         <f t="shared" si="9"/>
         <v>13</v>
       </c>
-      <c r="U13" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T13,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V13" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T13,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U13,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W13" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U13,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
-    <row r="14" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>24</v>
       </c>
@@ -1573,79 +1618,82 @@
         <v>20000000000</v>
       </c>
       <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="4" t="s">
+      <c r="D14" s="5">
+        <v>30000000000</v>
+      </c>
+      <c r="E14" s="2"/>
+      <c r="F14" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="7" t="str">
+      <c r="G14" s="2"/>
+      <c r="H14" s="7" t="str">
         <f t="shared" si="2"/>
         <v/>
       </c>
-      <c r="H14" s="10" t="s">
+      <c r="I14" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="I14" s="10" t="s">
+      <c r="J14" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="J14" s="10" t="s">
+      <c r="K14" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="K14" s="12" t="str">
+      <c r="L14" s="12" t="str">
         <f t="shared" si="3"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\ARBA\2023\02\</v>
       </c>
-      <c r="L14" s="12" t="str">
+      <c r="M14" s="12" t="str">
         <f t="shared" si="4"/>
         <v>C:\Users\Agustin Bustos\Desktop\Test\Cliente 4\RETPER\AGIP\2023\02\</v>
       </c>
-      <c r="M14" s="11">
+      <c r="N14" s="11">
         <v>44958</v>
       </c>
-      <c r="N14" s="9" t="str">
+      <c r="O14" s="9" t="str">
         <f t="shared" si="5"/>
         <v>02/2023</v>
       </c>
-      <c r="O14" s="9">
+      <c r="P14" s="9">
         <f t="shared" si="15"/>
         <v>2023</v>
       </c>
-      <c r="P14" s="9">
+      <c r="Q14" s="9">
         <f t="shared" si="16"/>
         <v>2</v>
       </c>
-      <c r="Q14" s="9">
+      <c r="R14" s="9">
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-      <c r="R14" s="9">
+      <c r="S14" s="9">
         <f t="shared" si="7"/>
         <v>1</v>
       </c>
-      <c r="S14" s="9" t="str">
+      <c r="T14" s="9" t="str">
         <f t="shared" si="8"/>
         <v>20000000000 - 202302 - Cliente 4</v>
       </c>
-      <c r="T14" s="9" t="str">
+      <c r="U14" s="9" t="str">
         <f t="shared" si="9"/>
         <v>14</v>
       </c>
-      <c r="U14" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T14,[1]ARBA!$A:$B,2,0),"")</f>
-        <v/>
-      </c>
       <c r="V14" s="9" t="str">
-        <f>IFERROR(VLOOKUP(T14,[1]AGIP!$A:$B,2,0),"")</f>
+        <f>IFERROR(VLOOKUP(U14,[1]ARBA!$A:$B,2,0),"")</f>
+        <v/>
+      </c>
+      <c r="W14" s="9" t="str">
+        <f>IFERROR(VLOOKUP(U14,[1]AGIP!$A:$B,2,0),"")</f>
         <v/>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:V14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E4">
+  <autoFilter ref="A1:W14" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:F4">
     <sortCondition ref="A2"/>
   </sortState>
-  <dataValidations count="1">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="I2:J14" xr:uid="{16927795-E0AC-4AAA-87BF-385CFC41B068}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="J2:K14" xr:uid="{16927795-E0AC-4AAA-87BF-385CFC41B068}">
       <formula1>"SI,NO"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>